<commit_message>
Adding a loader for the website
</commit_message>
<xml_diff>
--- a/Backend/Uploads/Wedding Products.xlsx
+++ b/Backend/Uploads/Wedding Products.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4505"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/keyideas/Downloads/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439FCDE4-996A-DC42-97C1-470AEB192722}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="20100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="504" windowWidth="23256" windowHeight="13176" tabRatio="345"/>
   </bookViews>
   <sheets>
     <sheet name="Wedding Bands" sheetId="2" r:id="rId1"/>
@@ -19,20 +13,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Wedding Bands'!$A$1:$AD$58</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="124519"/>
   <customWorkbookViews>
     <customWorkbookView name="Filter 1" guid="{AC5D767D-828D-4BE6-868E-8C5F71E75B81}" maximized="1" windowWidth="0" windowHeight="0" activeSheetId="0"/>
   </customWorkbookViews>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId11" roundtripDataSignature="AMtx7mguqbkVzXRaktIfIupsD0HqkDtuYg=="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="" roundtripDataSignature="AMtx7mguqbkVzXRaktIfIupsD0HqkDtuYg=="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="669" uniqueCount="318">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="284">
   <si>
     <t>prod_sku</t>
   </si>
@@ -241,9 +235,6 @@
     <t xml:space="preserve">White Gold </t>
   </si>
   <si>
-    <t>wedding-bands/127b01/shapes/round/127b01-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Engraved Diamond Wedding Band</t>
   </si>
   <si>
@@ -253,9 +244,6 @@
     <t>Diamond Men,White Gold Men,Men Wedding Band</t>
   </si>
   <si>
-    <t>wedding-bands/138a03/shapes/round/138a03-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Black Diamond Trim Wedding Band</t>
   </si>
   <si>
@@ -265,9 +253,6 @@
     <t>Black Diamond Men,White Gold Men,Platinum Men,Men Wedding Band</t>
   </si>
   <si>
-    <t>wedding-bands/178b01/shapes/round/178b01-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Diamond Wedding Band 1841G</t>
   </si>
   <si>
@@ -277,9 +262,6 @@
     <t>Diamond Men,White Gold Men,Yellow Gold Men,Rose Gold Men,Platinum Men,Men Wedding Band</t>
   </si>
   <si>
-    <t>wedding-bands/1841/shapes/round/1841-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>wedding-bands/1841/shapes/round/1841-rosegold_round_default.jpg</t>
   </si>
   <si>
@@ -292,9 +274,6 @@
     <t>A stunning Dora men's 3 row black diamond wedding band with rows of shared prong set black diamonds adorning the center for a stylish look that will turn heads.</t>
   </si>
   <si>
-    <t>wedding-bands/210b01/shapes/round/210b01-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's Simple Domed Wedding Band</t>
   </si>
   <si>
@@ -304,9 +283,6 @@
     <t>Tantalum Men,White Gold Men,Men Wedding Band</t>
   </si>
   <si>
-    <t>wedding-bands/292a25/shapes/round/292a25-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Diamond Men,White Gold Men,Two Tone Men,Platinum Men,Men Wedding Band</t>
   </si>
   <si>
@@ -322,9 +298,6 @@
     <t>Womens</t>
   </si>
   <si>
-    <t>wedding-bands/4345/shapes/round/4345-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>wedding-bands/4345/shapes/round/4345-rosegold_round_default.jpg</t>
   </si>
   <si>
@@ -337,9 +310,6 @@
     <t>A Dora men's trim wedding band with brushed tantalum and a simple center trim.</t>
   </si>
   <si>
-    <t>wedding-bands/533a02/shapes/round/533a02-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's Rose Gold Criss Cross Wedding Band</t>
   </si>
   <si>
@@ -358,18 +328,12 @@
     <t>This stunning Dora men's polished edge wedding band features brushed tantalum with polished edges, a classic you can never go wrong with.</t>
   </si>
   <si>
-    <t>wedding-bands/574a12/shapes/round/574a12-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Offset Black Diamond Wedding Band</t>
   </si>
   <si>
     <t>A classic Dora men's offset black diamond wedding band with a brushed white gold finish and a thin offset trim of black diamonds.</t>
   </si>
   <si>
-    <t>wedding-bands/577a11/shapes/round/577a11-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Mens Black Wedding Band</t>
   </si>
   <si>
@@ -391,18 +355,12 @@
     <t>Carbon Fiber Men,White Gold Men,Men Wedding Band</t>
   </si>
   <si>
-    <t>wedding-bands/588b00/shapes/round/588b00-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's Modern Wedding Band</t>
   </si>
   <si>
     <t>A modern yet timeless Dora men's wedding band featuring white gold and a carbon fiber trim that you can never go wrong with.</t>
   </si>
   <si>
-    <t>wedding-bands/589b00/shapes/round/589b00-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's Rose Gold Wedding Band</t>
   </si>
   <si>
@@ -421,9 +379,6 @@
     <t>0.6ct.</t>
   </si>
   <si>
-    <t>wedding-bands/592a00/shapes/round/592a00-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's Beveled Edge Rose Gold Wedding Band</t>
   </si>
   <si>
@@ -439,18 +394,12 @@
     <t>This modern Dora men's bezel diamond wedding band features carbon fiber with polished white gold detailing and a round diamond. The perfect ratio of sleek and classy.</t>
   </si>
   <si>
-    <t>wedding-bands/592b02/shapes/round/592b02-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's 3 Stone Bezel Diamond Wedding Band</t>
   </si>
   <si>
     <t>This beautiful Dora men's 3 stone bezel diamond wedding band features carbon fiber and white gold with 3 bezel set diamonds.</t>
   </si>
   <si>
-    <t>wedding-bands/592b03/shapes/round/592b03-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's Thick Rose Gold Wedding Band</t>
   </si>
   <si>
@@ -511,18 +460,12 @@
     <t>0.144ct.</t>
   </si>
   <si>
-    <t>wedding-bands/599a00/shapes/round/599a00-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Angled Channel Diamond Wedding Band</t>
   </si>
   <si>
     <t>This Dora men's angled channel diamond wedding band features an angled slot channel set with round diamonds.</t>
   </si>
   <si>
-    <t>wedding-bands/606a03/shapes/round/606a03-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Diamond Men,Two Tone Men,Men Wedding Band</t>
   </si>
   <si>
@@ -538,9 +481,6 @@
     <t>0.58ct.</t>
   </si>
   <si>
-    <t>wedding-bands/6094lbd/shapes/round/6094lbd-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's Carbon Fiber And Rose Gold Trim Wedding Band</t>
   </si>
   <si>
@@ -556,27 +496,18 @@
     <t>A beautiful Dora men's brushed inlay wedding band featuring shiny polished tantalum with a contrasting brushed inlay. This ring exhibits the perfect balance of sleek and class.</t>
   </si>
   <si>
-    <t>wedding-bands/622a09/shapes/round/622a09-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's White Gold And Carbon Fiber Trim Wedding Band</t>
   </si>
   <si>
     <t>This Dora men's white gold and carbon fiber trim wedding band features tantalum and brushed carbon fiber trims with a polished white gold center.</t>
   </si>
   <si>
-    <t>wedding-bands/626a04/shapes/round/626a04-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's Domed Brushed Wedding Band</t>
   </si>
   <si>
     <t>A modern Dora men's domed brushed wedding band featuring brushed tantalum that will never go out of style.</t>
   </si>
   <si>
-    <t>wedding-bands/631b06/shapes/round/631b06-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Two Tone Trim Diamond Wedding Band</t>
   </si>
   <si>
@@ -607,9 +538,6 @@
     <t>This three row diamond wedding band features channel set diamonds in the center surrounded by two rows of pave set diamonds and a milgrain finish for a stunning look.</t>
   </si>
   <si>
-    <t>wedding-bands/6502/shapes/round/6502-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>wedding-bands/6502/shapes/round/6502-rosegold_round_default.jpg</t>
   </si>
   <si>
@@ -625,12 +553,6 @@
     <t>Blue Diamond Women,Channel Women,White Gold Women,Platinum Women,Women Wedding Band</t>
   </si>
   <si>
-    <t>wedding-bands/6502lbd/shapes/round/three-row-blue-and-white-diamond-wedding-band.jpg</t>
-  </si>
-  <si>
-    <t>wedding-bands/6502lbd/shapes/round/three-row-blue-and-white-diamond-wedding-band-on-hand.jpg,wedding-bands/6502lbd/shapes/round/three-row-blue-and-white-diamond-wedding-band-on-hand2.jpg</t>
-  </si>
-  <si>
     <t>Three Row Black And White Diamond Wedding Band</t>
   </si>
   <si>
@@ -640,18 +562,12 @@
     <t>Black Diamond Women,Channel Women,White Gold Women,Platinum Women,Women Wedding Band</t>
   </si>
   <si>
-    <t>wedding-bands/6502lbk/shapes/round/three-row-black-and-white-diamond-wedding-band.jpg</t>
-  </si>
-  <si>
     <t>Men's Textured Wedding Band</t>
   </si>
   <si>
     <t>This Dora men's textured wedding band features a beautiful polished white gold band with a textured carbon fiber center.</t>
   </si>
   <si>
-    <t>wedding-bands/650b01/shapes/round/650b01-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Mens Gold Diamond Wedding Band</t>
   </si>
   <si>
@@ -661,9 +577,6 @@
     <t>10.8 Grams</t>
   </si>
   <si>
-    <t>wedding-bands/6548g/shapes/round/6548g-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>wedding-bands/6548g/shapes/round/6548g-rosegold_round_default.jpg</t>
   </si>
   <si>
@@ -685,27 +598,18 @@
     <t>This Dora men's domed wedding band shows off a gorgeous brushed carbon fiber with a contrasting white gold strip running across the center.</t>
   </si>
   <si>
-    <t>wedding-bands/657b00/shapes/round/657b00-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Simple Black Diamond Wedding Band</t>
   </si>
   <si>
     <t>This Dora men's simple black diamond wedding band features a polished slim trim in the middle adorned with 8 black diamonds.</t>
   </si>
   <si>
-    <t>wedding-bands/664b00/shapes/round/664b00-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Hammered Black Diamond Wedding Band</t>
   </si>
   <si>
     <t>A beautiful Dora men's hammered black diamond wedding band with a stunning hammered finish and black diamonds decorating the center.</t>
   </si>
   <si>
-    <t>wedding-bands/665b00/shapes/round/665b00-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's Inlay Diamond Wedding Band</t>
   </si>
   <si>
@@ -715,9 +619,6 @@
     <t>0.119ct.</t>
   </si>
   <si>
-    <t>wedding-bands/667b00/shapes/round/667b00-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's Black Diamond Wedding Band</t>
   </si>
   <si>
@@ -727,18 +628,12 @@
     <t>Carbon Fiber Men,White Gold Men,Men Wedding Band,Black Diamond Men</t>
   </si>
   <si>
-    <t>wedding-bands/668b00/shapes/round/668b00-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's Black Diamond Trim Wedding Band</t>
   </si>
   <si>
     <t>This captivating Dora men's black diamond trim wedding band features carbon fiber and a white gold trim with 5 gorgeous black diamonds.</t>
   </si>
   <si>
-    <t>wedding-bands/669b00/shapes/round/669b00-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Men's Yellow Gold And Black Diamond Wedding Band</t>
   </si>
   <si>
@@ -757,9 +652,6 @@
     <t>A classy Dora men's asymmetrical wedding band with brushed carbon fiber and white gold.</t>
   </si>
   <si>
-    <t>wedding-bands/671b00/shapes/round/671b00-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Unique Ornate Wedding Band</t>
   </si>
   <si>
@@ -769,9 +661,6 @@
     <t>Diamond Women,White Gold Women,Tri Color Women,Platinum Women,Women Wedding Band</t>
   </si>
   <si>
-    <t>wedding-bands/6723/shapes/round/6723-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>wedding-bands/6723/shapes/round/6723-whitegold_platinum_round_1.jpg</t>
   </si>
   <si>
@@ -793,9 +682,6 @@
     <t>15 Grams</t>
   </si>
   <si>
-    <t>wedding-bands/6842g/shapes/round/6842g-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>wedding-bands/6842g/shapes/round/6842g-whitegold_yellow_round_default.jpg</t>
   </si>
   <si>
@@ -811,9 +697,6 @@
     <t>14.3 Grams</t>
   </si>
   <si>
-    <t>wedding-bands/6921g/shapes/round/6921g-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Mens Inlay Wedding Band</t>
   </si>
   <si>
@@ -823,9 +706,6 @@
     <t>15.3 Grams</t>
   </si>
   <si>
-    <t>wedding-bands/6923g/shapes/round/6923g-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>wedding-bands/6923g/shapes/round/6923g-whitegold_yellow_round_default.jpg</t>
   </si>
   <si>
@@ -844,9 +724,6 @@
     <t>White Gold, WRG, WYG, Tri Color</t>
   </si>
   <si>
-    <t>wedding-bands/6950/shapes/round/6950-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>wedding-bands/6950/shapes/round/6950-whitegold_platinum_round_1.jpg,wedding-bands/6950/shapes/round/6950-whitegold_platinum_round_2.jpg</t>
   </si>
   <si>
@@ -868,9 +745,6 @@
     <t>Black Diamond Women,White Gold Women,Platinum Women,Women Wedding Band</t>
   </si>
   <si>
-    <t>wedding-bands/6950lbk/shapes/round/6950lbk-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>Unique Trim Wedding Band</t>
   </si>
   <si>
@@ -880,9 +754,6 @@
     <t>Tri Color Women,White Gold Women,Platinum Women,Women Wedding Band</t>
   </si>
   <si>
-    <t>wedding-bands/6986l/shapes/round/6986l-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>wedding-bands/6986l/shapes/round/6986l-tricolor_round_default.jpg</t>
   </si>
   <si>
@@ -892,9 +763,6 @@
     <t>This beautiful wavy wedding band features 2 channel set diamonds with a unique wavy design and pave set diamonds for extra sparkle.</t>
   </si>
   <si>
-    <t>wedding-bands/7001/shapes/round/7001-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>wedding-bands/7001/shapes/round/7001-whitegold_yellow_round_default.jpg</t>
   </si>
   <si>
@@ -910,9 +778,6 @@
     <t>A unique vintage diamond wedding band featuring a round center with a crossing section pave set with diamonds and two larger channel set diamond accents. The outer ridges are also adorned with diamonds along with a milgrain finish for a touch of elegance.</t>
   </si>
   <si>
-    <t>wedding-bands/7014l/shapes/round/7014l-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>wedding-bands/7014l/shapes/round/7014l-tricolor_round_default.jpg</t>
   </si>
   <si>
@@ -928,9 +793,6 @@
     <t>0.98ct.</t>
   </si>
   <si>
-    <t>wedding-bands/7016l/shapes/round/7016l-whitegold_platinum_round_default.jpg</t>
-  </si>
-  <si>
     <t>wedding-bands/7016l/shapes/round/7016l-whitegold_rose_round_default.jpg</t>
   </si>
   <si>
@@ -986,13 +848,43 @@
   </si>
   <si>
     <t>You can use your own images and update its path in the CSV</t>
+  </si>
+  <si>
+    <t>https://cdn.shopify.com/s/files/1/0263/9695/0581/products/B0009YELLOW.jpg?v=1681330636</t>
+  </si>
+  <si>
+    <t>https://www.exclusivelydiamonds.com/public/1.0/uploads/source/brands/memoire/4670035_0.jpg</t>
+  </si>
+  <si>
+    <t>rating</t>
+  </si>
+  <si>
+    <t>rating_count</t>
+  </si>
+  <si>
+    <t>https://www.dercodiamonds.com/wp-content/uploads/2022/02/GR027-R03-WG0.jpg</t>
+  </si>
+  <si>
+    <t>https://www.dercodiamonds.com/wp-content/uploads/2023/01/SingleprongRBBG_LY.jpg</t>
+  </si>
+  <si>
+    <t>https://www.dercodiamonds.com/wp-content/uploads/2020/04/723204_yg_4.jpg</t>
+  </si>
+  <si>
+    <t>https://www.dercodiamonds.com/wp-content/uploads/2023/01/CompassHiddenHalo_RP-768x768.jpg</t>
+  </si>
+  <si>
+    <t>https://www.dercodiamonds.com/wp-content/uploads/2020/04/TIFFSTYLE_yg_4-768x768.jpg</t>
+  </si>
+  <si>
+    <t>https://www.dercodiamonds.com/wp-content/uploads/2024/04/760494_WF.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1019,6 +911,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12.3"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1028,7 +940,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -1079,11 +991,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1111,8 +1051,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="4">
@@ -1364,54 +1316,54 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FF4A86E8"/>
   </sheetPr>
-  <dimension ref="A1:AD58"/>
+  <dimension ref="A1:AF60"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="112" zoomScaleNormal="112" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="S2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D38" sqref="D38"/>
+      <selection pane="bottomRight" activeCell="S19" sqref="S19:S25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="16.33203125" customWidth="1"/>
-    <col min="2" max="2" width="23.5" style="8" customWidth="1"/>
-    <col min="3" max="3" width="56.5" customWidth="1"/>
+    <col min="2" max="2" width="23.44140625" style="8" customWidth="1"/>
+    <col min="3" max="3" width="56.44140625" customWidth="1"/>
     <col min="4" max="4" width="71.6640625" customWidth="1"/>
-    <col min="5" max="5" width="17.5" customWidth="1"/>
-    <col min="6" max="6" width="112.1640625" customWidth="1"/>
-    <col min="7" max="7" width="12.83203125" customWidth="1"/>
-    <col min="8" max="8" width="8.1640625" customWidth="1"/>
-    <col min="9" max="9" width="13.1640625" customWidth="1"/>
-    <col min="10" max="10" width="6.5" customWidth="1"/>
-    <col min="11" max="11" width="9.5" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="112.109375" customWidth="1"/>
+    <col min="7" max="7" width="12.77734375" customWidth="1"/>
+    <col min="8" max="8" width="8.109375" customWidth="1"/>
+    <col min="9" max="9" width="13.109375" customWidth="1"/>
+    <col min="10" max="10" width="6.44140625" customWidth="1"/>
+    <col min="11" max="11" width="9.44140625" customWidth="1"/>
     <col min="12" max="12" width="14.33203125" customWidth="1"/>
     <col min="13" max="13" width="7" customWidth="1"/>
-    <col min="14" max="14" width="22.83203125" customWidth="1"/>
-    <col min="15" max="15" width="35.1640625" customWidth="1"/>
+    <col min="14" max="14" width="22.77734375" customWidth="1"/>
+    <col min="15" max="15" width="35.109375" customWidth="1"/>
     <col min="16" max="16" width="8.6640625" customWidth="1"/>
-    <col min="17" max="17" width="39.5" customWidth="1"/>
-    <col min="18" max="18" width="9.1640625" customWidth="1"/>
+    <col min="17" max="17" width="39.44140625" customWidth="1"/>
+    <col min="18" max="18" width="9.109375" customWidth="1"/>
     <col min="19" max="19" width="76" customWidth="1"/>
     <col min="20" max="20" width="80.6640625" customWidth="1"/>
-    <col min="21" max="21" width="34.5" customWidth="1"/>
-    <col min="22" max="22" width="27.83203125" customWidth="1"/>
-    <col min="23" max="23" width="37.5" customWidth="1"/>
-    <col min="24" max="24" width="29.5" customWidth="1"/>
-    <col min="25" max="25" width="43.5" customWidth="1"/>
+    <col min="21" max="21" width="34.44140625" customWidth="1"/>
+    <col min="22" max="22" width="27.77734375" customWidth="1"/>
+    <col min="23" max="23" width="37.44140625" customWidth="1"/>
+    <col min="24" max="24" width="29.44140625" customWidth="1"/>
+    <col min="25" max="25" width="43.44140625" customWidth="1"/>
     <col min="26" max="26" width="36.33203125" customWidth="1"/>
-    <col min="27" max="27" width="43.5" customWidth="1"/>
-    <col min="28" max="28" width="34.1640625" customWidth="1"/>
-    <col min="29" max="29" width="35.83203125" customWidth="1"/>
-    <col min="30" max="30" width="31.1640625" customWidth="1"/>
+    <col min="27" max="27" width="43.44140625" customWidth="1"/>
+    <col min="28" max="28" width="34.109375" customWidth="1"/>
+    <col min="29" max="29" width="35.77734375" customWidth="1"/>
+    <col min="30" max="30" width="31.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:32" ht="18" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1502,13 +1454,19 @@
       <c r="AD1" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE1" s="19" t="s">
+        <v>276</v>
+      </c>
+      <c r="AF1" s="19" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A2" s="4">
         <v>1001</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C2" s="4" t="s">
         <v>63</v>
@@ -1548,8 +1506,8 @@
         <v>68</v>
       </c>
       <c r="R2" s="7"/>
-      <c r="S2" s="4" t="s">
-        <v>69</v>
+      <c r="S2" s="21" t="s">
+        <v>275</v>
       </c>
       <c r="T2" s="4"/>
       <c r="U2" s="4"/>
@@ -1562,25 +1520,31 @@
       <c r="AB2" s="5"/>
       <c r="AC2" s="5"/>
       <c r="AD2" s="5"/>
-    </row>
-    <row r="3" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE2" s="20">
+        <v>4.2</v>
+      </c>
+      <c r="AF2" s="20">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A3" s="4">
         <v>1002</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C3" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D3" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="E3" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F3" s="7" t="s">
         <v>71</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>72</v>
       </c>
       <c r="G3" s="5" t="s">
         <v>67</v>
@@ -1612,8 +1576,8 @@
         <v>68</v>
       </c>
       <c r="R3" s="7"/>
-      <c r="S3" s="4" t="s">
-        <v>73</v>
+      <c r="S3" s="22" t="s">
+        <v>278</v>
       </c>
       <c r="T3" s="4"/>
       <c r="U3" s="4"/>
@@ -1626,25 +1590,31 @@
       <c r="AB3" s="5"/>
       <c r="AC3" s="5"/>
       <c r="AD3" s="5"/>
-    </row>
-    <row r="4" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE3" s="20">
+        <v>3.1</v>
+      </c>
+      <c r="AF3" s="20">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A4" s="4">
         <v>1003</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C4" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="F4" s="7" t="s">
         <v>74</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>76</v>
       </c>
       <c r="G4" s="5" t="s">
         <v>67</v>
@@ -1674,8 +1644,8 @@
       <c r="R4" s="7">
         <v>2450</v>
       </c>
-      <c r="S4" s="4" t="s">
-        <v>77</v>
+      <c r="S4" s="22" t="s">
+        <v>279</v>
       </c>
       <c r="T4" s="4"/>
       <c r="U4" s="4"/>
@@ -1688,25 +1658,31 @@
       <c r="AB4" s="5"/>
       <c r="AC4" s="5"/>
       <c r="AD4" s="5"/>
-    </row>
-    <row r="5" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE4" s="20">
+        <v>3.9</v>
+      </c>
+      <c r="AF4" s="20">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A5" s="4">
         <v>1004</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E5" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G5" s="5" t="s">
         <v>67</v>
@@ -1742,16 +1718,16 @@
       <c r="R5" s="7">
         <v>3975</v>
       </c>
-      <c r="S5" s="9" t="s">
-        <v>81</v>
+      <c r="S5" s="22" t="s">
+        <v>280</v>
       </c>
       <c r="T5" s="4"/>
       <c r="U5" s="9" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="V5" s="4"/>
       <c r="W5" s="9" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="X5" s="5"/>
       <c r="Y5" s="4"/>
@@ -1760,19 +1736,25 @@
       <c r="AB5" s="5"/>
       <c r="AC5" s="5"/>
       <c r="AD5" s="5"/>
-    </row>
-    <row r="6" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE5" s="20">
+        <v>3</v>
+      </c>
+      <c r="AF5" s="20">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A6" s="4">
         <v>1005</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>65</v>
@@ -1806,8 +1788,8 @@
         <v>68</v>
       </c>
       <c r="R6" s="7"/>
-      <c r="S6" s="4" t="s">
-        <v>86</v>
+      <c r="S6" s="22" t="s">
+        <v>274</v>
       </c>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
@@ -1820,25 +1802,31 @@
       <c r="AB6" s="5"/>
       <c r="AC6" s="5"/>
       <c r="AD6" s="5"/>
-    </row>
-    <row r="7" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE6" s="20">
+        <v>3.9</v>
+      </c>
+      <c r="AF6" s="20">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A7" s="4">
         <v>1006</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E7" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G7" s="5" t="s">
         <v>67</v>
@@ -1860,8 +1848,8 @@
       <c r="P7" s="7"/>
       <c r="Q7" s="5"/>
       <c r="R7" s="7"/>
-      <c r="S7" s="6" t="s">
-        <v>90</v>
+      <c r="S7" s="22" t="s">
+        <v>281</v>
       </c>
       <c r="T7" s="4"/>
       <c r="U7" s="4"/>
@@ -1874,28 +1862,34 @@
       <c r="AB7" s="5"/>
       <c r="AC7" s="5"/>
       <c r="AD7" s="5"/>
-    </row>
-    <row r="8" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE7" s="20">
+        <v>3</v>
+      </c>
+      <c r="AF7" s="20">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A8" s="4">
         <v>1007</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H8" s="7">
         <v>8</v>
@@ -1928,16 +1922,16 @@
       <c r="R8" s="7">
         <v>2890</v>
       </c>
-      <c r="S8" s="9" t="s">
-        <v>96</v>
+      <c r="S8" s="23" t="s">
+        <v>282</v>
       </c>
       <c r="T8" s="4"/>
       <c r="U8" s="9" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="V8" s="4"/>
       <c r="W8" s="9" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="X8" s="5"/>
       <c r="Y8" s="4"/>
@@ -1946,25 +1940,31 @@
       <c r="AB8" s="5"/>
       <c r="AC8" s="5"/>
       <c r="AD8" s="5"/>
-    </row>
-    <row r="9" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE8" s="20">
+        <v>4</v>
+      </c>
+      <c r="AF8" s="20">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="9" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A9" s="4">
         <v>1008</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E9" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G9" s="5" t="s">
         <v>67</v>
@@ -1986,8 +1986,8 @@
       <c r="P9" s="7"/>
       <c r="Q9" s="5"/>
       <c r="R9" s="7"/>
-      <c r="S9" s="6" t="s">
-        <v>101</v>
+      <c r="S9" s="21" t="s">
+        <v>275</v>
       </c>
       <c r="T9" s="4"/>
       <c r="U9" s="4"/>
@@ -2000,25 +2000,31 @@
       <c r="AB9" s="5"/>
       <c r="AC9" s="5"/>
       <c r="AD9" s="5"/>
-    </row>
-    <row r="10" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE9" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF9" s="20">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A10" s="4">
         <v>1009</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="E10" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G10" s="5" t="s">
         <v>67</v>
@@ -2040,10 +2046,12 @@
       <c r="P10" s="7"/>
       <c r="Q10" s="5"/>
       <c r="R10" s="7"/>
-      <c r="S10" s="4"/>
+      <c r="S10" s="22" t="s">
+        <v>278</v>
+      </c>
       <c r="T10" s="4"/>
       <c r="U10" s="4" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
@@ -2054,25 +2062,31 @@
       <c r="AB10" s="5"/>
       <c r="AC10" s="5"/>
       <c r="AD10" s="5"/>
-    </row>
-    <row r="11" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE10" s="20">
+        <v>4.2</v>
+      </c>
+      <c r="AF10" s="20">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A11" s="4">
         <v>1010</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="E11" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G11" s="5" t="s">
         <v>67</v>
@@ -2094,8 +2108,8 @@
       <c r="P11" s="7"/>
       <c r="Q11" s="5"/>
       <c r="R11" s="7"/>
-      <c r="S11" s="6" t="s">
-        <v>108</v>
+      <c r="S11" s="22" t="s">
+        <v>279</v>
       </c>
       <c r="T11" s="4"/>
       <c r="U11" s="4"/>
@@ -2108,19 +2122,25 @@
       <c r="AB11" s="5"/>
       <c r="AC11" s="5"/>
       <c r="AD11" s="5"/>
-    </row>
-    <row r="12" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE11" s="20">
+        <v>4</v>
+      </c>
+      <c r="AF11" s="20">
+        <v>912</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A12" s="4">
         <v>1011</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E12" s="6" t="s">
         <v>65</v>
@@ -2154,8 +2174,8 @@
         <v>68</v>
       </c>
       <c r="R12" s="7"/>
-      <c r="S12" s="4" t="s">
-        <v>111</v>
+      <c r="S12" s="22" t="s">
+        <v>280</v>
       </c>
       <c r="T12" s="4"/>
       <c r="U12" s="4"/>
@@ -2168,25 +2188,31 @@
       <c r="AB12" s="5"/>
       <c r="AC12" s="5"/>
       <c r="AD12" s="5"/>
-    </row>
-    <row r="13" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE12" s="20">
+        <v>4</v>
+      </c>
+      <c r="AF12" s="20">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A13" s="4">
         <v>1012</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>112</v>
+        <v>102</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
       <c r="E13" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="G13" s="5" t="s">
         <v>67</v>
@@ -2208,12 +2234,14 @@
       <c r="P13" s="7"/>
       <c r="Q13" s="5"/>
       <c r="R13" s="7"/>
-      <c r="S13" s="4"/>
+      <c r="S13" s="22" t="s">
+        <v>274</v>
+      </c>
       <c r="T13" s="4"/>
       <c r="U13" s="4"/>
       <c r="V13" s="4"/>
       <c r="W13" s="4" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="X13" s="5"/>
       <c r="Y13" s="4"/>
@@ -2222,25 +2250,31 @@
       <c r="AB13" s="5"/>
       <c r="AC13" s="5"/>
       <c r="AD13" s="5"/>
-    </row>
-    <row r="14" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE13" s="20">
+        <v>4</v>
+      </c>
+      <c r="AF13" s="20">
+        <v>1200</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A14" s="4">
         <v>1013</v>
       </c>
       <c r="B14" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>116</v>
+        <v>106</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>67</v>
@@ -2262,8 +2296,8 @@
       <c r="P14" s="7"/>
       <c r="Q14" s="5"/>
       <c r="R14" s="7"/>
-      <c r="S14" s="4" t="s">
-        <v>119</v>
+      <c r="S14" s="22" t="s">
+        <v>281</v>
       </c>
       <c r="T14" s="4"/>
       <c r="U14" s="4"/>
@@ -2276,25 +2310,31 @@
       <c r="AB14" s="5"/>
       <c r="AC14" s="5"/>
       <c r="AD14" s="5"/>
-    </row>
-    <row r="15" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE14" s="20">
+        <v>4</v>
+      </c>
+      <c r="AF14" s="20">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A15" s="4">
         <v>1014</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>120</v>
+        <v>109</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G15" s="5" t="s">
         <v>67</v>
@@ -2316,8 +2356,8 @@
       <c r="P15" s="7"/>
       <c r="Q15" s="5"/>
       <c r="R15" s="7"/>
-      <c r="S15" s="4" t="s">
-        <v>122</v>
+      <c r="S15" s="23" t="s">
+        <v>282</v>
       </c>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
@@ -2330,25 +2370,31 @@
       <c r="AB15" s="5"/>
       <c r="AC15" s="5"/>
       <c r="AD15" s="5"/>
-    </row>
-    <row r="16" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE15" s="20">
+        <v>3.7</v>
+      </c>
+      <c r="AF15" s="20">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="16" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A16" s="4">
         <v>1015</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>123</v>
+        <v>111</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G16" s="5" t="s">
         <v>67</v>
@@ -2370,10 +2416,12 @@
       <c r="P16" s="7"/>
       <c r="Q16" s="5"/>
       <c r="R16" s="7"/>
-      <c r="S16" s="4"/>
+      <c r="S16" s="17" t="s">
+        <v>275</v>
+      </c>
       <c r="T16" s="4"/>
       <c r="U16" s="4" t="s">
-        <v>125</v>
+        <v>113</v>
       </c>
       <c r="V16" s="4"/>
       <c r="W16" s="4"/>
@@ -2384,25 +2432,31 @@
       <c r="AB16" s="5"/>
       <c r="AC16" s="5"/>
       <c r="AD16" s="5"/>
-    </row>
-    <row r="17" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE16" s="20">
+        <v>3.8</v>
+      </c>
+      <c r="AF16" s="20">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A17" s="4">
         <v>1016</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>126</v>
+        <v>114</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G17" s="5" t="s">
         <v>67</v>
@@ -2415,7 +2469,7 @@
         <v>6</v>
       </c>
       <c r="K17" s="7" t="s">
-        <v>128</v>
+        <v>116</v>
       </c>
       <c r="L17" s="7" t="s">
         <v>30</v>
@@ -2434,8 +2488,8 @@
         <v>68</v>
       </c>
       <c r="R17" s="7"/>
-      <c r="S17" s="4" t="s">
-        <v>129</v>
+      <c r="S17" s="17" t="s">
+        <v>274</v>
       </c>
       <c r="T17" s="4"/>
       <c r="U17" s="4"/>
@@ -2448,25 +2502,31 @@
       <c r="AB17" s="5"/>
       <c r="AC17" s="5"/>
       <c r="AD17" s="5"/>
-    </row>
-    <row r="18" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE17" s="20">
+        <v>3.9</v>
+      </c>
+      <c r="AF17" s="20">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A18" s="4">
         <v>1017</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>130</v>
+        <v>117</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>131</v>
+        <v>118</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G18" s="5" t="s">
         <v>67</v>
@@ -2488,10 +2548,12 @@
       <c r="P18" s="7"/>
       <c r="Q18" s="5"/>
       <c r="R18" s="7"/>
-      <c r="S18" s="4"/>
+      <c r="S18" s="17" t="s">
+        <v>275</v>
+      </c>
       <c r="T18" s="4"/>
       <c r="U18" s="4" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="V18" s="4"/>
       <c r="W18" s="4"/>
@@ -2502,25 +2564,31 @@
       <c r="AB18" s="5"/>
       <c r="AC18" s="5"/>
       <c r="AD18" s="5"/>
-    </row>
-    <row r="19" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE18" s="20">
+        <v>3</v>
+      </c>
+      <c r="AF18" s="20">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A19" s="4">
         <v>1018</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>134</v>
+        <v>121</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G19" s="5" t="s">
         <v>67</v>
@@ -2548,8 +2616,8 @@
       <c r="P19" s="7"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="7"/>
-      <c r="S19" s="4" t="s">
-        <v>135</v>
+      <c r="S19" s="21" t="s">
+        <v>275</v>
       </c>
       <c r="T19" s="4"/>
       <c r="U19" s="4"/>
@@ -2562,25 +2630,31 @@
       <c r="AB19" s="5"/>
       <c r="AC19" s="5"/>
       <c r="AD19" s="5"/>
-    </row>
-    <row r="20" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE19" s="20">
+        <v>2</v>
+      </c>
+      <c r="AF19" s="20">
+        <v>986</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A20" s="4">
         <v>1019</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="E20" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G20" s="5" t="s">
         <v>67</v>
@@ -2608,8 +2682,8 @@
       <c r="P20" s="7"/>
       <c r="Q20" s="5"/>
       <c r="R20" s="7"/>
-      <c r="S20" s="4" t="s">
-        <v>138</v>
+      <c r="S20" s="22" t="s">
+        <v>278</v>
       </c>
       <c r="T20" s="4"/>
       <c r="U20" s="4"/>
@@ -2622,25 +2696,31 @@
       <c r="AB20" s="5"/>
       <c r="AC20" s="5"/>
       <c r="AD20" s="5"/>
-    </row>
-    <row r="21" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE20" s="20">
+        <v>2</v>
+      </c>
+      <c r="AF20" s="20">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A21" s="4">
         <v>1020</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>140</v>
+        <v>125</v>
       </c>
       <c r="E21" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G21" s="5" t="s">
         <v>67</v>
@@ -2662,10 +2742,12 @@
       <c r="P21" s="7"/>
       <c r="Q21" s="5"/>
       <c r="R21" s="7"/>
-      <c r="S21" s="4"/>
+      <c r="S21" s="22" t="s">
+        <v>279</v>
+      </c>
       <c r="T21" s="4"/>
       <c r="U21" s="4" t="s">
-        <v>141</v>
+        <v>126</v>
       </c>
       <c r="V21" s="4"/>
       <c r="W21" s="4"/>
@@ -2676,25 +2758,31 @@
       <c r="AB21" s="5"/>
       <c r="AC21" s="5"/>
       <c r="AD21" s="5"/>
-    </row>
-    <row r="22" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE21" s="20">
+        <v>2.6</v>
+      </c>
+      <c r="AF21" s="20">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="22" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A22" s="4">
         <v>1021</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>142</v>
+        <v>127</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>143</v>
+        <v>128</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="G22" s="5" t="s">
         <v>67</v>
@@ -2722,12 +2810,14 @@
       <c r="P22" s="7"/>
       <c r="Q22" s="5"/>
       <c r="R22" s="7"/>
-      <c r="S22" s="4"/>
+      <c r="S22" s="22" t="s">
+        <v>280</v>
+      </c>
       <c r="T22" s="4"/>
       <c r="U22" s="4"/>
       <c r="V22" s="4"/>
       <c r="W22" s="4" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="X22" s="5"/>
       <c r="Y22" s="4"/>
@@ -2736,25 +2826,31 @@
       <c r="AB22" s="5"/>
       <c r="AC22" s="5"/>
       <c r="AD22" s="5"/>
-    </row>
-    <row r="23" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE22" s="20">
+        <v>2.7</v>
+      </c>
+      <c r="AF22" s="20">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="23" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A23" s="4">
         <v>1022</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>145</v>
+        <v>130</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>146</v>
+        <v>131</v>
       </c>
       <c r="E23" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="G23" s="5" t="s">
         <v>67</v>
@@ -2776,10 +2872,12 @@
       <c r="P23" s="7"/>
       <c r="Q23" s="5"/>
       <c r="R23" s="7"/>
-      <c r="S23" s="4"/>
+      <c r="S23" s="22" t="s">
+        <v>274</v>
+      </c>
       <c r="T23" s="4"/>
       <c r="U23" s="6" t="s">
-        <v>148</v>
+        <v>133</v>
       </c>
       <c r="V23" s="4"/>
       <c r="W23" s="4"/>
@@ -2790,25 +2888,31 @@
       <c r="AB23" s="5"/>
       <c r="AC23" s="5"/>
       <c r="AD23" s="5"/>
-    </row>
-    <row r="24" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE23" s="20">
+        <v>2.9</v>
+      </c>
+      <c r="AF23" s="20">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="24" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A24" s="4">
         <v>1023</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>149</v>
+        <v>134</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="E24" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="G24" s="5" t="s">
         <v>67</v>
@@ -2830,10 +2934,12 @@
       <c r="P24" s="7"/>
       <c r="Q24" s="5"/>
       <c r="R24" s="7"/>
-      <c r="S24" s="4"/>
+      <c r="S24" s="22" t="s">
+        <v>281</v>
+      </c>
       <c r="T24" s="4"/>
       <c r="U24" s="4" t="s">
-        <v>151</v>
+        <v>136</v>
       </c>
       <c r="V24" s="4"/>
       <c r="W24" s="4"/>
@@ -2844,25 +2950,31 @@
       <c r="AB24" s="5"/>
       <c r="AC24" s="5"/>
       <c r="AD24" s="5"/>
-    </row>
-    <row r="25" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE24" s="20">
+        <v>2.1</v>
+      </c>
+      <c r="AF24" s="20">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="25" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A25" s="4">
         <v>1024</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>152</v>
+        <v>137</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>153</v>
+        <v>138</v>
       </c>
       <c r="E25" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="G25" s="5" t="s">
         <v>67</v>
@@ -2884,12 +2996,14 @@
       <c r="P25" s="7"/>
       <c r="Q25" s="5"/>
       <c r="R25" s="7"/>
-      <c r="S25" s="4"/>
+      <c r="S25" s="23" t="s">
+        <v>282</v>
+      </c>
       <c r="T25" s="4"/>
       <c r="U25" s="4"/>
       <c r="V25" s="4"/>
       <c r="W25" s="4" t="s">
-        <v>154</v>
+        <v>139</v>
       </c>
       <c r="X25" s="5"/>
       <c r="Y25" s="4"/>
@@ -2898,25 +3012,31 @@
       <c r="AB25" s="5"/>
       <c r="AC25" s="5"/>
       <c r="AD25" s="5"/>
-    </row>
-    <row r="26" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE25" s="20">
+        <v>2</v>
+      </c>
+      <c r="AF25" s="20">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="26" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A26" s="4">
         <v>1025</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>155</v>
+        <v>140</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>156</v>
+        <v>141</v>
       </c>
       <c r="E26" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="G26" s="5" t="s">
         <v>67</v>
@@ -2929,7 +3049,7 @@
         <v>12</v>
       </c>
       <c r="K26" s="7" t="s">
-        <v>158</v>
+        <v>143</v>
       </c>
       <c r="L26" s="7" t="s">
         <v>30</v>
@@ -2950,8 +3070,8 @@
       <c r="R26" s="7">
         <v>3665</v>
       </c>
-      <c r="S26" s="4" t="s">
-        <v>159</v>
+      <c r="S26" s="17" t="s">
+        <v>278</v>
       </c>
       <c r="T26" s="4"/>
       <c r="U26" s="4"/>
@@ -2964,25 +3084,31 @@
       <c r="AB26" s="5"/>
       <c r="AC26" s="5"/>
       <c r="AD26" s="5"/>
-    </row>
-    <row r="27" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE26" s="20">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="AF26" s="20">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="27" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A27" s="4">
         <v>1026</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>161</v>
+        <v>145</v>
       </c>
       <c r="E27" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="G27" s="5" t="s">
         <v>67</v>
@@ -3016,8 +3142,8 @@
       <c r="R27" s="7">
         <v>3165</v>
       </c>
-      <c r="S27" s="4" t="s">
-        <v>162</v>
+      <c r="S27" s="17" t="s">
+        <v>279</v>
       </c>
       <c r="T27" s="4"/>
       <c r="U27" s="4"/>
@@ -3030,28 +3156,34 @@
       <c r="AB27" s="5"/>
       <c r="AC27" s="5"/>
       <c r="AD27" s="5"/>
-    </row>
-    <row r="28" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE27" s="20">
+        <v>2.5</v>
+      </c>
+      <c r="AF27" s="20">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="28" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A28" s="4">
         <v>1027</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>164</v>
+        <v>147</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>165</v>
+        <v>148</v>
       </c>
       <c r="E28" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H28" s="7">
         <v>28</v>
@@ -3063,7 +3195,7 @@
         <v>30</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>167</v>
+        <v>150</v>
       </c>
       <c r="L28" s="7" t="s">
         <v>30</v>
@@ -3086,8 +3218,8 @@
       <c r="R28" s="7">
         <v>7250</v>
       </c>
-      <c r="S28" s="4" t="s">
-        <v>168</v>
+      <c r="S28" s="17" t="s">
+        <v>280</v>
       </c>
       <c r="T28" s="4"/>
       <c r="U28" s="4"/>
@@ -3100,25 +3232,31 @@
       <c r="AB28" s="5"/>
       <c r="AC28" s="5"/>
       <c r="AD28" s="5"/>
-    </row>
-    <row r="29" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE28" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF28" s="20">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="29" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A29" s="4">
         <v>1028</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>169</v>
+        <v>151</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>170</v>
+        <v>152</v>
       </c>
       <c r="E29" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="G29" s="5" t="s">
         <v>67</v>
@@ -3140,10 +3278,12 @@
       <c r="P29" s="7"/>
       <c r="Q29" s="5"/>
       <c r="R29" s="7"/>
-      <c r="S29" s="4"/>
+      <c r="S29" s="17" t="s">
+        <v>274</v>
+      </c>
       <c r="T29" s="4"/>
       <c r="U29" s="6" t="s">
-        <v>171</v>
+        <v>153</v>
       </c>
       <c r="V29" s="4"/>
       <c r="W29" s="4"/>
@@ -3154,25 +3294,31 @@
       <c r="AB29" s="5"/>
       <c r="AC29" s="5"/>
       <c r="AD29" s="5"/>
-    </row>
-    <row r="30" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE29" s="20">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="AF29" s="20">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="30" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A30" s="4">
         <v>1029</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>172</v>
+        <v>154</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>173</v>
+        <v>155</v>
       </c>
       <c r="E30" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G30" s="5" t="s">
         <v>67</v>
@@ -3194,8 +3340,8 @@
       <c r="P30" s="7"/>
       <c r="Q30" s="5"/>
       <c r="R30" s="7"/>
-      <c r="S30" s="6" t="s">
-        <v>174</v>
+      <c r="S30" s="18" t="s">
+        <v>281</v>
       </c>
       <c r="T30" s="4"/>
       <c r="U30" s="4"/>
@@ -3208,25 +3354,31 @@
       <c r="AB30" s="5"/>
       <c r="AC30" s="5"/>
       <c r="AD30" s="5"/>
-    </row>
-    <row r="31" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE30" s="20">
+        <v>3.7</v>
+      </c>
+      <c r="AF30" s="20">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="31" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A31" s="4">
         <v>1030</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>175</v>
+        <v>156</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>176</v>
+        <v>157</v>
       </c>
       <c r="E31" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G31" s="5" t="s">
         <v>67</v>
@@ -3248,8 +3400,8 @@
       <c r="P31" s="7"/>
       <c r="Q31" s="5"/>
       <c r="R31" s="7"/>
-      <c r="S31" s="4" t="s">
-        <v>177</v>
+      <c r="S31" s="17" t="s">
+        <v>282</v>
       </c>
       <c r="T31" s="4"/>
       <c r="U31" s="4"/>
@@ -3262,25 +3414,31 @@
       <c r="AB31" s="5"/>
       <c r="AC31" s="5"/>
       <c r="AD31" s="5"/>
-    </row>
-    <row r="32" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE31" s="20">
+        <v>4.2</v>
+      </c>
+      <c r="AF31" s="20">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="32" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A32" s="4">
         <v>1031</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="E32" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="G32" s="5" t="s">
         <v>67</v>
@@ -3302,8 +3460,8 @@
       <c r="P32" s="7"/>
       <c r="Q32" s="5"/>
       <c r="R32" s="7"/>
-      <c r="S32" s="6" t="s">
-        <v>180</v>
+      <c r="S32" s="18" t="s">
+        <v>283</v>
       </c>
       <c r="T32" s="4"/>
       <c r="U32" s="4"/>
@@ -3316,25 +3474,31 @@
       <c r="AB32" s="5"/>
       <c r="AC32" s="5"/>
       <c r="AD32" s="5"/>
-    </row>
-    <row r="33" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE32" s="20">
+        <v>4</v>
+      </c>
+      <c r="AF32" s="20">
+        <v>985</v>
+      </c>
+    </row>
+    <row r="33" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A33" s="4">
         <v>1032</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>181</v>
+        <v>160</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>182</v>
+        <v>161</v>
       </c>
       <c r="E33" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>163</v>
+        <v>146</v>
       </c>
       <c r="G33" s="5" t="s">
         <v>67</v>
@@ -3366,39 +3530,47 @@
         <v>38</v>
       </c>
       <c r="R33" s="7"/>
-      <c r="S33" s="4"/>
+      <c r="S33" s="17" t="s">
+        <v>275</v>
+      </c>
       <c r="T33" s="4"/>
       <c r="U33" s="4"/>
       <c r="V33" s="4"/>
       <c r="W33" s="4"/>
       <c r="X33" s="5"/>
       <c r="Y33" s="4" t="s">
-        <v>183</v>
+        <v>162</v>
       </c>
       <c r="Z33" s="5"/>
       <c r="AA33" s="5"/>
       <c r="AB33" s="5"/>
       <c r="AC33" s="5"/>
       <c r="AD33" s="5"/>
-    </row>
-    <row r="34" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE33" s="20">
+        <v>3.9</v>
+      </c>
+      <c r="AF33" s="20">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="34" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A34" s="4">
         <v>1033</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>184</v>
+        <v>163</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>185</v>
+        <v>164</v>
       </c>
       <c r="E34" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>186</v>
+        <v>165</v>
       </c>
       <c r="G34" s="5" t="s">
         <v>67</v>
@@ -3415,12 +3587,14 @@
         <v>675</v>
       </c>
       <c r="O34" s="5" t="s">
-        <v>187</v>
+        <v>166</v>
       </c>
       <c r="P34" s="7"/>
       <c r="Q34" s="5"/>
       <c r="R34" s="7"/>
-      <c r="S34" s="4"/>
+      <c r="S34" s="17" t="s">
+        <v>278</v>
+      </c>
       <c r="T34" s="4"/>
       <c r="U34" s="4"/>
       <c r="V34" s="4"/>
@@ -3429,33 +3603,39 @@
       <c r="Y34" s="4"/>
       <c r="Z34" s="5"/>
       <c r="AA34" s="6" t="s">
-        <v>188</v>
+        <v>167</v>
       </c>
       <c r="AB34" s="5"/>
       <c r="AC34" s="5"/>
       <c r="AD34" s="5"/>
-    </row>
-    <row r="35" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE34" s="20">
+        <v>3.5</v>
+      </c>
+      <c r="AF34" s="20">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="35" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A35" s="4">
         <v>1034</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>189</v>
+        <v>168</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>190</v>
+        <v>169</v>
       </c>
       <c r="E35" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H35" s="7">
         <v>15</v>
@@ -3488,16 +3668,16 @@
       <c r="R35" s="7">
         <v>4525</v>
       </c>
-      <c r="S35" s="4" t="s">
-        <v>191</v>
+      <c r="S35" s="17" t="s">
+        <v>279</v>
       </c>
       <c r="T35" s="4"/>
       <c r="U35" s="4" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="V35" s="4"/>
       <c r="W35" s="4" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="X35" s="5"/>
       <c r="Y35" s="4"/>
@@ -3506,28 +3686,34 @@
       <c r="AB35" s="5"/>
       <c r="AC35" s="5"/>
       <c r="AD35" s="5"/>
-    </row>
-    <row r="36" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE35" s="20">
+        <v>4</v>
+      </c>
+      <c r="AF35" s="20">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="36" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A36" s="4">
         <v>1035</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="E36" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H36" s="7">
         <v>16</v>
@@ -3562,12 +3748,10 @@
       <c r="R36" s="7">
         <v>4610</v>
       </c>
-      <c r="S36" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="T36" s="4" t="s">
-        <v>198</v>
-      </c>
+      <c r="S36" s="17" t="s">
+        <v>280</v>
+      </c>
+      <c r="T36" s="4"/>
       <c r="U36" s="4"/>
       <c r="V36" s="4"/>
       <c r="W36" s="4"/>
@@ -3578,28 +3762,34 @@
       <c r="AB36" s="5"/>
       <c r="AC36" s="5"/>
       <c r="AD36" s="5"/>
-    </row>
-    <row r="37" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE36" s="20">
+        <v>3.6</v>
+      </c>
+      <c r="AF36" s="20">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="37" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A37" s="4">
         <v>1036</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>199</v>
+        <v>175</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>200</v>
+        <v>176</v>
       </c>
       <c r="E37" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H37" s="7">
         <v>17</v>
@@ -3634,8 +3824,8 @@
       <c r="R37" s="7">
         <v>4150</v>
       </c>
-      <c r="S37" s="4" t="s">
-        <v>202</v>
+      <c r="S37" s="17" t="s">
+        <v>274</v>
       </c>
       <c r="T37" s="4"/>
       <c r="U37" s="4"/>
@@ -3648,25 +3838,31 @@
       <c r="AB37" s="5"/>
       <c r="AC37" s="5"/>
       <c r="AD37" s="5"/>
-    </row>
-    <row r="38" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE37" s="20">
+        <v>3.7</v>
+      </c>
+      <c r="AF37" s="20">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="38" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A38" s="4">
         <v>1037</v>
       </c>
       <c r="B38" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>203</v>
+        <v>178</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>204</v>
+        <v>179</v>
       </c>
       <c r="E38" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G38" s="5" t="s">
         <v>67</v>
@@ -3688,8 +3884,8 @@
       <c r="P38" s="7"/>
       <c r="Q38" s="5"/>
       <c r="R38" s="7"/>
-      <c r="S38" s="4" t="s">
-        <v>205</v>
+      <c r="S38" s="17" t="s">
+        <v>281</v>
       </c>
       <c r="T38" s="4"/>
       <c r="U38" s="4"/>
@@ -3702,25 +3898,31 @@
       <c r="AB38" s="5"/>
       <c r="AC38" s="5"/>
       <c r="AD38" s="5"/>
-    </row>
-    <row r="39" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE38" s="20">
+        <v>3.8</v>
+      </c>
+      <c r="AF38" s="20">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A39" s="4">
         <v>1038</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
       <c r="E39" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="G39" s="5" t="s">
         <v>67</v>
@@ -3729,7 +3931,7 @@
         <v>19</v>
       </c>
       <c r="I39" s="7" t="s">
-        <v>208</v>
+        <v>182</v>
       </c>
       <c r="J39" s="7">
         <v>1</v>
@@ -3756,16 +3958,16 @@
       <c r="R39" s="7">
         <v>3685</v>
       </c>
-      <c r="S39" s="6" t="s">
-        <v>209</v>
+      <c r="S39" s="18" t="s">
+        <v>282</v>
       </c>
       <c r="T39" s="4"/>
       <c r="U39" s="4" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="V39" s="4"/>
       <c r="W39" s="4" t="s">
-        <v>211</v>
+        <v>184</v>
       </c>
       <c r="X39" s="5"/>
       <c r="Y39" s="4"/>
@@ -3774,25 +3976,31 @@
       <c r="AB39" s="5"/>
       <c r="AC39" s="5"/>
       <c r="AD39" s="5"/>
-    </row>
-    <row r="40" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE39" s="20">
+        <v>4</v>
+      </c>
+      <c r="AF39" s="20">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="40" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A40" s="4">
         <v>1039</v>
       </c>
       <c r="B40" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>212</v>
+        <v>185</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>213</v>
+        <v>186</v>
       </c>
       <c r="E40" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>147</v>
+        <v>132</v>
       </c>
       <c r="G40" s="5" t="s">
         <v>67</v>
@@ -3814,10 +4022,12 @@
       <c r="P40" s="7"/>
       <c r="Q40" s="5"/>
       <c r="R40" s="7"/>
-      <c r="S40" s="4"/>
+      <c r="S40" s="17" t="s">
+        <v>275</v>
+      </c>
       <c r="T40" s="4"/>
       <c r="U40" s="6" t="s">
-        <v>214</v>
+        <v>187</v>
       </c>
       <c r="V40" s="4"/>
       <c r="W40" s="4"/>
@@ -3828,25 +4038,31 @@
       <c r="AB40" s="5"/>
       <c r="AC40" s="5"/>
       <c r="AD40" s="5"/>
-    </row>
-    <row r="41" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE40" s="20">
+        <v>4.3</v>
+      </c>
+      <c r="AF40" s="20">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="41" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A41" s="4">
         <v>1040</v>
       </c>
       <c r="B41" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>215</v>
+        <v>188</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>216</v>
+        <v>189</v>
       </c>
       <c r="E41" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G41" s="5" t="s">
         <v>67</v>
@@ -3868,8 +4084,8 @@
       <c r="P41" s="7"/>
       <c r="Q41" s="5"/>
       <c r="R41" s="7"/>
-      <c r="S41" s="4" t="s">
-        <v>217</v>
+      <c r="S41" s="17" t="s">
+        <v>278</v>
       </c>
       <c r="T41" s="4"/>
       <c r="U41" s="4"/>
@@ -3882,25 +4098,31 @@
       <c r="AB41" s="5"/>
       <c r="AC41" s="5"/>
       <c r="AD41" s="5"/>
-    </row>
-    <row r="42" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE41" s="20">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="AF41" s="20">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="42" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A42" s="4">
         <v>1041</v>
       </c>
       <c r="B42" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>218</v>
+        <v>190</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>219</v>
+        <v>191</v>
       </c>
       <c r="E42" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G42" s="5" t="s">
         <v>67</v>
@@ -3930,8 +4152,8 @@
       <c r="R42" s="7">
         <v>2565</v>
       </c>
-      <c r="S42" s="4" t="s">
-        <v>220</v>
+      <c r="S42" s="17" t="s">
+        <v>279</v>
       </c>
       <c r="T42" s="4"/>
       <c r="U42" s="4"/>
@@ -3944,19 +4166,25 @@
       <c r="AB42" s="5"/>
       <c r="AC42" s="5"/>
       <c r="AD42" s="5"/>
-    </row>
-    <row r="43" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE42" s="20">
+        <v>4</v>
+      </c>
+      <c r="AF42" s="20">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="43" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A43" s="4">
         <v>1042</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>221</v>
+        <v>192</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>222</v>
+        <v>193</v>
       </c>
       <c r="E43" s="6" t="s">
         <v>65</v>
@@ -3990,8 +4218,8 @@
         <v>68</v>
       </c>
       <c r="R43" s="7"/>
-      <c r="S43" s="4" t="s">
-        <v>223</v>
+      <c r="S43" s="17" t="s">
+        <v>280</v>
       </c>
       <c r="T43" s="4"/>
       <c r="U43" s="4"/>
@@ -4004,25 +4232,31 @@
       <c r="AB43" s="5"/>
       <c r="AC43" s="5"/>
       <c r="AD43" s="5"/>
-    </row>
-    <row r="44" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE43" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF43" s="20">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="44" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A44" s="4">
         <v>1043</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>224</v>
+        <v>194</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>225</v>
+        <v>195</v>
       </c>
       <c r="E44" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G44" s="5" t="s">
         <v>67</v>
@@ -4035,7 +4269,7 @@
         <v>7</v>
       </c>
       <c r="K44" s="4" t="s">
-        <v>226</v>
+        <v>196</v>
       </c>
       <c r="L44" s="7" t="s">
         <v>30</v>
@@ -4050,8 +4284,8 @@
       <c r="P44" s="7"/>
       <c r="Q44" s="5"/>
       <c r="R44" s="7"/>
-      <c r="S44" s="4" t="s">
-        <v>227</v>
+      <c r="S44" s="17" t="s">
+        <v>274</v>
       </c>
       <c r="T44" s="4"/>
       <c r="U44" s="4"/>
@@ -4064,25 +4298,31 @@
       <c r="AB44" s="5"/>
       <c r="AC44" s="5"/>
       <c r="AD44" s="5"/>
-    </row>
-    <row r="45" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE44" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF44" s="20">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="45" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A45" s="4">
         <v>1044</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>228</v>
+        <v>197</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>229</v>
+        <v>198</v>
       </c>
       <c r="E45" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="G45" s="5" t="s">
         <v>67</v>
@@ -4106,8 +4346,8 @@
       <c r="P45" s="7"/>
       <c r="Q45" s="5"/>
       <c r="R45" s="7"/>
-      <c r="S45" s="4" t="s">
-        <v>231</v>
+      <c r="S45" s="17" t="s">
+        <v>281</v>
       </c>
       <c r="T45" s="4"/>
       <c r="U45" s="4"/>
@@ -4120,25 +4360,31 @@
       <c r="AB45" s="5"/>
       <c r="AC45" s="5"/>
       <c r="AD45" s="5"/>
-    </row>
-    <row r="46" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE45" s="20">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="AF45" s="20">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A46" s="4">
         <v>1045</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="E46" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>230</v>
+        <v>199</v>
       </c>
       <c r="G46" s="5" t="s">
         <v>67</v>
@@ -4162,8 +4408,8 @@
       <c r="P46" s="7"/>
       <c r="Q46" s="5"/>
       <c r="R46" s="7"/>
-      <c r="S46" s="4" t="s">
-        <v>234</v>
+      <c r="S46" s="18" t="s">
+        <v>282</v>
       </c>
       <c r="T46" s="4"/>
       <c r="U46" s="4"/>
@@ -4176,25 +4422,31 @@
       <c r="AB46" s="5"/>
       <c r="AC46" s="5"/>
       <c r="AD46" s="5"/>
-    </row>
-    <row r="47" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE46" s="20">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="AF46" s="20">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A47" s="4">
         <v>1046</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>235</v>
+        <v>202</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>236</v>
+        <v>203</v>
       </c>
       <c r="E47" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>237</v>
+        <v>204</v>
       </c>
       <c r="G47" s="5" t="s">
         <v>67</v>
@@ -4218,12 +4470,14 @@
       <c r="P47" s="7"/>
       <c r="Q47" s="5"/>
       <c r="R47" s="7"/>
-      <c r="S47" s="4"/>
+      <c r="S47" s="17" t="s">
+        <v>275</v>
+      </c>
       <c r="T47" s="4"/>
       <c r="U47" s="4"/>
       <c r="V47" s="4"/>
       <c r="W47" s="7" t="s">
-        <v>238</v>
+        <v>205</v>
       </c>
       <c r="X47" s="5"/>
       <c r="Y47" s="4"/>
@@ -4232,25 +4486,31 @@
       <c r="AB47" s="5"/>
       <c r="AC47" s="5"/>
       <c r="AD47" s="5"/>
-    </row>
-    <row r="48" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE47" s="20">
+        <v>4</v>
+      </c>
+      <c r="AF47" s="20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="48" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A48" s="4">
         <v>1047</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>239</v>
+        <v>206</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>240</v>
+        <v>207</v>
       </c>
       <c r="E48" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G48" s="5" t="s">
         <v>67</v>
@@ -4272,8 +4532,8 @@
       <c r="P48" s="7"/>
       <c r="Q48" s="5"/>
       <c r="R48" s="7"/>
-      <c r="S48" s="4" t="s">
-        <v>241</v>
+      <c r="S48" s="17" t="s">
+        <v>278</v>
       </c>
       <c r="T48" s="4"/>
       <c r="U48" s="4"/>
@@ -4286,28 +4546,34 @@
       <c r="AB48" s="5"/>
       <c r="AC48" s="5"/>
       <c r="AD48" s="5"/>
-    </row>
-    <row r="49" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE48" s="20">
+        <v>3.8</v>
+      </c>
+      <c r="AF48" s="20">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="49" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A49" s="4">
         <v>1048</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>242</v>
+        <v>208</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>243</v>
+        <v>209</v>
       </c>
       <c r="E49" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H49" s="7">
         <v>13</v>
@@ -4340,11 +4606,11 @@
       <c r="R49" s="7">
         <v>7080</v>
       </c>
-      <c r="S49" s="9" t="s">
-        <v>245</v>
+      <c r="S49" s="17" t="s">
+        <v>279</v>
       </c>
       <c r="T49" s="9" t="s">
-        <v>246</v>
+        <v>211</v>
       </c>
       <c r="U49" s="4"/>
       <c r="V49" s="4"/>
@@ -4355,30 +4621,36 @@
       <c r="AA49" s="5"/>
       <c r="AB49" s="5"/>
       <c r="AC49" s="9" t="s">
-        <v>247</v>
+        <v>212</v>
       </c>
       <c r="AD49" s="9" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="50" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+        <v>213</v>
+      </c>
+      <c r="AE49" s="20">
+        <v>3.8</v>
+      </c>
+      <c r="AF49" s="20">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="50" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A50" s="4">
         <v>1049</v>
       </c>
       <c r="B50" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>250</v>
+        <v>215</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>251</v>
+        <v>216</v>
       </c>
       <c r="E50" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G50" s="5" t="s">
         <v>67</v>
@@ -4387,7 +4659,7 @@
         <v>14</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>252</v>
+        <v>217</v>
       </c>
       <c r="J50" s="7">
         <v>1</v>
@@ -4414,8 +4686,8 @@
       <c r="R50" s="7">
         <v>5080</v>
       </c>
-      <c r="S50" s="4" t="s">
-        <v>253</v>
+      <c r="S50" s="17" t="s">
+        <v>280</v>
       </c>
       <c r="T50" s="4"/>
       <c r="U50" s="4"/>
@@ -4423,34 +4695,40 @@
       <c r="W50" s="4"/>
       <c r="X50" s="5"/>
       <c r="Y50" s="4" t="s">
-        <v>254</v>
+        <v>218</v>
       </c>
       <c r="Z50" s="5"/>
       <c r="AA50" s="4" t="s">
-        <v>255</v>
+        <v>219</v>
       </c>
       <c r="AB50" s="5"/>
       <c r="AC50" s="5"/>
       <c r="AD50" s="5"/>
-    </row>
-    <row r="51" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE50" s="20">
+        <v>3.8</v>
+      </c>
+      <c r="AF50" s="20">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="51" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A51" s="4">
         <v>1050</v>
       </c>
       <c r="B51" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>256</v>
+        <v>220</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>257</v>
+        <v>221</v>
       </c>
       <c r="E51" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>157</v>
+        <v>142</v>
       </c>
       <c r="G51" s="5" t="s">
         <v>67</v>
@@ -4459,7 +4737,7 @@
         <v>15</v>
       </c>
       <c r="I51" s="7" t="s">
-        <v>258</v>
+        <v>222</v>
       </c>
       <c r="J51" s="7">
         <v>2</v>
@@ -4486,8 +4764,8 @@
       <c r="R51" s="7">
         <v>5110</v>
       </c>
-      <c r="S51" s="6" t="s">
-        <v>259</v>
+      <c r="S51" s="17" t="s">
+        <v>274</v>
       </c>
       <c r="T51" s="4"/>
       <c r="U51" s="4"/>
@@ -4500,25 +4778,31 @@
       <c r="AB51" s="5"/>
       <c r="AC51" s="5"/>
       <c r="AD51" s="5"/>
-    </row>
-    <row r="52" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE51" s="20">
+        <v>3</v>
+      </c>
+      <c r="AF51" s="20">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="52" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A52" s="4">
         <v>1051</v>
       </c>
       <c r="B52" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>260</v>
+        <v>223</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>261</v>
+        <v>224</v>
       </c>
       <c r="E52" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F52" s="7" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="G52" s="5" t="s">
         <v>67</v>
@@ -4527,7 +4811,7 @@
         <v>16</v>
       </c>
       <c r="I52" s="7" t="s">
-        <v>262</v>
+        <v>225</v>
       </c>
       <c r="J52" s="7">
         <v>1</v>
@@ -4554,8 +4838,8 @@
       <c r="R52" s="7">
         <v>5545</v>
       </c>
-      <c r="S52" s="4" t="s">
-        <v>263</v>
+      <c r="S52" s="17" t="s">
+        <v>281</v>
       </c>
       <c r="T52" s="4"/>
       <c r="U52" s="4"/>
@@ -4563,37 +4847,43 @@
       <c r="W52" s="4"/>
       <c r="X52" s="5"/>
       <c r="Y52" s="6" t="s">
-        <v>264</v>
+        <v>226</v>
       </c>
       <c r="Z52" s="5"/>
       <c r="AA52" s="4" t="s">
-        <v>265</v>
+        <v>227</v>
       </c>
       <c r="AB52" s="5"/>
       <c r="AC52" s="5"/>
       <c r="AD52" s="5"/>
-    </row>
-    <row r="53" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE52" s="20">
+        <v>3.2</v>
+      </c>
+      <c r="AF52" s="20">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="53" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A53" s="4">
         <v>1052</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C53" s="7" t="s">
-        <v>266</v>
+        <v>228</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>267</v>
+        <v>229</v>
       </c>
       <c r="E53" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F53" s="7" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H53" s="7">
         <v>17</v>
@@ -4615,61 +4905,67 @@
         <v>2065</v>
       </c>
       <c r="O53" s="5" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="P53" s="7">
         <v>2590</v>
       </c>
       <c r="Q53" s="5" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="R53" s="7">
         <v>3060</v>
       </c>
-      <c r="S53" s="9" t="s">
-        <v>270</v>
+      <c r="S53" s="18" t="s">
+        <v>282</v>
       </c>
       <c r="T53" s="4" t="s">
-        <v>271</v>
+        <v>232</v>
       </c>
       <c r="U53" s="4"/>
       <c r="V53" s="4"/>
       <c r="W53" s="4"/>
       <c r="X53" s="5"/>
       <c r="Y53" s="9" t="s">
-        <v>272</v>
+        <v>233</v>
       </c>
       <c r="Z53" s="5"/>
       <c r="AA53" s="9" t="s">
-        <v>273</v>
+        <v>234</v>
       </c>
       <c r="AB53" s="5"/>
       <c r="AC53" s="9" t="s">
-        <v>274</v>
+        <v>235</v>
       </c>
       <c r="AD53" s="5"/>
-    </row>
-    <row r="54" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE53" s="20">
+        <v>3.6</v>
+      </c>
+      <c r="AF53" s="20">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="54" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A54" s="4">
         <v>1053</v>
       </c>
       <c r="B54" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>275</v>
+        <v>236</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>276</v>
+        <v>237</v>
       </c>
       <c r="E54" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F54" s="7" t="s">
-        <v>277</v>
+        <v>238</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H54" s="7">
         <v>18</v>
@@ -4704,8 +5000,8 @@
       <c r="R54" s="7">
         <v>3855</v>
       </c>
-      <c r="S54" s="6" t="s">
-        <v>278</v>
+      <c r="S54" s="17" t="s">
+        <v>275</v>
       </c>
       <c r="T54" s="4"/>
       <c r="U54" s="4"/>
@@ -4718,28 +5014,34 @@
       <c r="AB54" s="5"/>
       <c r="AC54" s="5"/>
       <c r="AD54" s="5"/>
-    </row>
-    <row r="55" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE54" s="20">
+        <v>3</v>
+      </c>
+      <c r="AF54" s="20">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="55" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A55" s="4">
         <v>1054</v>
       </c>
       <c r="B55" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>279</v>
+        <v>239</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>280</v>
+        <v>240</v>
       </c>
       <c r="E55" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F55" s="7" t="s">
-        <v>281</v>
+        <v>241</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H55" s="7">
         <v>19</v>
@@ -4772,8 +5074,8 @@
       <c r="R55" s="7">
         <v>6845</v>
       </c>
-      <c r="S55" s="6" t="s">
-        <v>282</v>
+      <c r="S55" s="17" t="s">
+        <v>278</v>
       </c>
       <c r="T55" s="4"/>
       <c r="U55" s="4"/>
@@ -4785,37 +5087,43 @@
       <c r="AA55" s="5"/>
       <c r="AB55" s="5"/>
       <c r="AC55" s="6" t="s">
-        <v>283</v>
+        <v>242</v>
       </c>
       <c r="AD55" s="5"/>
-    </row>
-    <row r="56" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE55" s="20">
+        <v>3.9</v>
+      </c>
+      <c r="AF55" s="20">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="56" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A56" s="4">
         <v>1055</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>284</v>
+        <v>243</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>285</v>
+        <v>244</v>
       </c>
       <c r="E56" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F56" s="7" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H56" s="7">
         <v>20</v>
       </c>
       <c r="I56" s="7" t="s">
-        <v>249</v>
+        <v>214</v>
       </c>
       <c r="J56" s="7">
         <v>18</v>
@@ -4831,19 +5139,19 @@
         <v>3740</v>
       </c>
       <c r="O56" s="5" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="P56" s="7">
         <v>4580</v>
       </c>
       <c r="Q56" s="5" t="s">
-        <v>269</v>
+        <v>231</v>
       </c>
       <c r="R56" s="7">
         <v>5345</v>
       </c>
-      <c r="S56" s="9" t="s">
-        <v>286</v>
+      <c r="S56" s="17" t="s">
+        <v>279</v>
       </c>
       <c r="T56" s="4"/>
       <c r="U56" s="4"/>
@@ -4851,39 +5159,45 @@
       <c r="W56" s="4"/>
       <c r="X56" s="5"/>
       <c r="Y56" s="9" t="s">
-        <v>287</v>
+        <v>245</v>
       </c>
       <c r="Z56" s="5"/>
       <c r="AA56" s="9" t="s">
-        <v>288</v>
+        <v>246</v>
       </c>
       <c r="AB56" s="5"/>
       <c r="AC56" s="9" t="s">
-        <v>289</v>
+        <v>247</v>
       </c>
       <c r="AD56" s="5"/>
-    </row>
-    <row r="57" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE56" s="20">
+        <v>4</v>
+      </c>
+      <c r="AF56" s="20">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="57" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A57" s="4">
         <v>1056</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>290</v>
+        <v>248</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>291</v>
+        <v>249</v>
       </c>
       <c r="E57" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F57" s="7" t="s">
-        <v>244</v>
+        <v>210</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H57" s="7">
         <v>21</v>
@@ -4916,8 +5230,8 @@
       <c r="R57" s="7">
         <v>7420</v>
       </c>
-      <c r="S57" s="6" t="s">
-        <v>292</v>
+      <c r="S57" s="17" t="s">
+        <v>280</v>
       </c>
       <c r="T57" s="4"/>
       <c r="U57" s="4"/>
@@ -4929,31 +5243,37 @@
       <c r="AA57" s="5"/>
       <c r="AB57" s="5"/>
       <c r="AC57" s="6" t="s">
-        <v>293</v>
+        <v>250</v>
       </c>
       <c r="AD57" s="5"/>
-    </row>
-    <row r="58" spans="1:30" s="8" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AE57" s="20">
+        <v>4.8</v>
+      </c>
+      <c r="AF57" s="20">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="58" spans="1:32" s="8" customFormat="1" ht="16.8">
       <c r="A58" s="4">
         <v>1057</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>294</v>
+        <v>251</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>295</v>
+        <v>252</v>
       </c>
       <c r="E58" s="6" t="s">
         <v>65</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>296</v>
+        <v>253</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="H58" s="7">
         <v>22</v>
@@ -4965,7 +5285,7 @@
         <v>85</v>
       </c>
       <c r="K58" s="7" t="s">
-        <v>297</v>
+        <v>254</v>
       </c>
       <c r="L58" s="7" t="s">
         <v>30</v>
@@ -4986,8 +5306,8 @@
       <c r="R58" s="7">
         <v>7865</v>
       </c>
-      <c r="S58" s="6" t="s">
-        <v>298</v>
+      <c r="S58" s="17" t="s">
+        <v>274</v>
       </c>
       <c r="T58" s="4"/>
       <c r="U58" s="4"/>
@@ -4997,11 +5317,23 @@
       <c r="Y58" s="4"/>
       <c r="Z58" s="5"/>
       <c r="AA58" s="6" t="s">
-        <v>299</v>
+        <v>255</v>
       </c>
       <c r="AB58" s="5"/>
       <c r="AC58" s="5"/>
       <c r="AD58" s="5"/>
+      <c r="AE58" s="20">
+        <v>5</v>
+      </c>
+      <c r="AF58" s="20">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="59" spans="1:32" ht="15" customHeight="1">
+      <c r="S59" s="17"/>
+    </row>
+    <row r="60" spans="1:32" ht="15" customHeight="1">
+      <c r="S60" s="18"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B58">
@@ -5014,13 +5346,72 @@
       <formula>COUNTIF(C:C,C1)&gt;1</formula>
     </cfRule>
   </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="S17" r:id="rId1"/>
+    <hyperlink ref="S16" r:id="rId2"/>
+    <hyperlink ref="S18" r:id="rId3"/>
+    <hyperlink ref="S26" r:id="rId4"/>
+    <hyperlink ref="S27" r:id="rId5"/>
+    <hyperlink ref="S28" r:id="rId6"/>
+    <hyperlink ref="S29" r:id="rId7"/>
+    <hyperlink ref="S30" r:id="rId8"/>
+    <hyperlink ref="S31" r:id="rId9"/>
+    <hyperlink ref="S32" r:id="rId10"/>
+    <hyperlink ref="S33" r:id="rId11"/>
+    <hyperlink ref="S34" r:id="rId12"/>
+    <hyperlink ref="S35" r:id="rId13"/>
+    <hyperlink ref="S36" r:id="rId14"/>
+    <hyperlink ref="S37" r:id="rId15"/>
+    <hyperlink ref="S38" r:id="rId16"/>
+    <hyperlink ref="S39" r:id="rId17"/>
+    <hyperlink ref="S40" r:id="rId18"/>
+    <hyperlink ref="S41" r:id="rId19"/>
+    <hyperlink ref="S42" r:id="rId20"/>
+    <hyperlink ref="S43" r:id="rId21"/>
+    <hyperlink ref="S44" r:id="rId22"/>
+    <hyperlink ref="S45" r:id="rId23"/>
+    <hyperlink ref="S46" r:id="rId24"/>
+    <hyperlink ref="S47" r:id="rId25"/>
+    <hyperlink ref="S48" r:id="rId26"/>
+    <hyperlink ref="S49" r:id="rId27"/>
+    <hyperlink ref="S50" r:id="rId28"/>
+    <hyperlink ref="S51" r:id="rId29"/>
+    <hyperlink ref="S52" r:id="rId30"/>
+    <hyperlink ref="S53" r:id="rId31"/>
+    <hyperlink ref="S54" r:id="rId32"/>
+    <hyperlink ref="S55" r:id="rId33"/>
+    <hyperlink ref="S56" r:id="rId34"/>
+    <hyperlink ref="S57" r:id="rId35"/>
+    <hyperlink ref="S58" r:id="rId36"/>
+    <hyperlink ref="S2" r:id="rId37"/>
+    <hyperlink ref="S3" r:id="rId38"/>
+    <hyperlink ref="S4" r:id="rId39"/>
+    <hyperlink ref="S5" r:id="rId40"/>
+    <hyperlink ref="S6" r:id="rId41"/>
+    <hyperlink ref="S7" r:id="rId42"/>
+    <hyperlink ref="S8" r:id="rId43"/>
+    <hyperlink ref="S9" r:id="rId44"/>
+    <hyperlink ref="S10" r:id="rId45"/>
+    <hyperlink ref="S11" r:id="rId46"/>
+    <hyperlink ref="S12" r:id="rId47"/>
+    <hyperlink ref="S13" r:id="rId48"/>
+    <hyperlink ref="S14" r:id="rId49"/>
+    <hyperlink ref="S15" r:id="rId50"/>
+    <hyperlink ref="S19" r:id="rId51"/>
+    <hyperlink ref="S20" r:id="rId52"/>
+    <hyperlink ref="S21" r:id="rId53"/>
+    <hyperlink ref="S22" r:id="rId54"/>
+    <hyperlink ref="S23" r:id="rId55"/>
+    <hyperlink ref="S24" r:id="rId56"/>
+    <hyperlink ref="S25" r:id="rId57"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{016A5CBF-4C6C-DB44-B2BC-4CBA4335083C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
@@ -5030,250 +5421,250 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="84.83203125" customWidth="1"/>
+    <col min="1" max="1" width="84.77734375" customWidth="1"/>
     <col min="2" max="2" width="70.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="15" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" s="12" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" s="13" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
       <c r="A5" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
       <c r="A6" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
       <c r="A7" s="11" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>307</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
       <c r="A8" s="13" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
       <c r="A9" s="11" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>309</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
       <c r="A10" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="16" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
       <c r="A11" s="11" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>310</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
       <c r="A12" s="11" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
       <c r="A13" s="13" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2">
       <c r="A14" s="13" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="15" t="s">
-        <v>313</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
       <c r="A15" s="11" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
       <c r="A16" s="13" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>315</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2">
       <c r="A17" s="11" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
       <c r="A18" s="13" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="15" t="s">
-        <v>316</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
       <c r="A19" s="14" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2">
       <c r="A20" s="14" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
       <c r="A21" s="14" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="15" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
       <c r="A22" s="14" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
       <c r="A23" s="14" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="15" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2">
       <c r="A24" s="14" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="15" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2">
       <c r="A25" s="14" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
       <c r="A26" s="14" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
       <c r="A27" s="14" t="s">
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2">
       <c r="A28" s="11" t="s">
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
       <c r="A29" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
       <c r="A30" s="11" t="s">
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>317</v>
+        <v>273</v>
       </c>
     </row>
   </sheetData>

</xml_diff>